<commit_message>
replaced mvr with mvc and removed box links from the treatment matrix
</commit_message>
<xml_diff>
--- a/docs/model_library/treatment_technology_matrix.xlsx
+++ b/docs/model_library/treatment_technology_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elmira\Documents\project-pareto\docs\model_library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE1EF8B-4F92-4889-8AF8-094427040398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB4E10B-971C-4C72-96E5-C92C1655AD0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="9" xr2:uid="{7EB8244F-7D23-43A8-881B-2A11527B8B6D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7EB8244F-7D23-43A8-881B-2A11527B8B6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="11" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="319">
   <si>
     <t>Pretreatment</t>
   </si>
@@ -425,9 +425,6 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Desalination and Reuse of High-Salinity Shale Gas Produced Water:
 Drivers, Technologies, and Future Directions</t>
   </si>
@@ -438,9 +435,6 @@
     <t>High level review/overview of mechanical vapor compression, membrane distillation, and forward osmosis as produced water desalination technologies</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1010792907327</t>
-  </si>
-  <si>
     <t>Energy consumption in desalinating produced water from shale oil and
 gas extraction</t>
   </si>
@@ -451,9 +445,6 @@
     <t>Thermo-economic analysis of MVC, MED, FO, HDH, MD, and hypothetical high-salinity RO</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1033462567339</t>
-  </si>
-  <si>
     <t>Optimal selection of an integrated produced water treatment system in the upstream of oil industry</t>
   </si>
   <si>
@@ -461,9 +452,6 @@
   </si>
   <si>
     <t>Superstructure optimization of produced water treatment systems</t>
-  </si>
-  <si>
-    <t>https://app.box.com/file/1032364724078</t>
   </si>
   <si>
     <t>Process optimization for zero-liquid discharge desalination of shale
@@ -476,9 +464,6 @@
     <t>Stochastic optimization of an MVC system with multiple evaporation effects</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1036511496497</t>
-  </si>
-  <si>
     <t>Shale gas flowback water desalination: Single vs multiple-effect evaporation with vapor recompression cycle and thermal integration</t>
   </si>
   <si>
@@ -488,9 +473,6 @@
     <t>Technoeconomic assessment of various configurations of MVC</t>
   </si>
   <si>
-    <t>https://app.box.com/file/953994391679</t>
-  </si>
-  <si>
     <t>Desalination of shale gas produced water: A rigorous design approach for zero-liquid discharge evaporation systems</t>
   </si>
   <si>
@@ -498,9 +480,6 @@
   </si>
   <si>
     <t>Technoeconomic assessment of single and double effect configurations of MVC, but with more rigorous heat transfer modeling compared to the above reference</t>
-  </si>
-  <si>
-    <t>https://app.box.com/file/953995037013</t>
   </si>
   <si>
     <t>Optimal Pretreatment System of Flowback Water from Shale Gas
@@ -513,9 +492,6 @@
     <t>Superstructure optimization of produced water pretreatment chains via GDP/MINLP formulation</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1036508861700</t>
-  </si>
-  <si>
     <t>Optimization of multistage membrane distillation system for treating shale gas produced water</t>
   </si>
   <si>
@@ -525,9 +501,6 @@
     <t>Technoeconomic assessment of multi-stage direct contact membrane distillation (DCMD)</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1036468183468</t>
-  </si>
-  <si>
     <t>Thermo-economic and environmental optimization of a solar-driven zero-liquid discharge system for shale gas wastewater desalination</t>
   </si>
   <si>
@@ -537,9 +510,6 @@
     <t>Technoecononomic assessment of MVC when using solar power to generate electricity. Multiobjective optimization with economic and enviromnental objectives.</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1036524459362</t>
-  </si>
-  <si>
     <t xml:space="preserve">Optimization-based modeling and economic comparison of membrane distillation configurations for application in shale gas produced water treatment </t>
   </si>
   <si>
@@ -549,9 +519,6 @@
     <t>Technoeconomic assessment of six different types of membrane distillation</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1017225945646</t>
-  </si>
-  <si>
     <t>Optimization-based modeling and analysis of brine reflux osmotically assisted reverse osmosis for application toward zero liquid discharge systems</t>
   </si>
   <si>
@@ -561,18 +528,12 @@
     <t>Technoeconomic assessment of OARO configurations</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1017245777730</t>
-  </si>
-  <si>
     <t>Optimization-based technoeconomic comparison of multi-stage membrane distillation configurations for hypersaline produced water desalination</t>
   </si>
   <si>
     <t>Cost optimization of several multi-stage MD configurations operating in continuous recirculation mode</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1042481307397</t>
-  </si>
-  <si>
     <t>Cost Optimization of Osmotically Assisted Reverse Osmosis</t>
   </si>
   <si>
@@ -582,9 +543,6 @@
     <t>Cost optimization of OARO</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1043487970790</t>
-  </si>
-  <si>
     <t>Pathways for minimal and zero liquid discharge with enhanced reverse osmosis technologies: Module-scale modeling and techno-economic assessment</t>
   </si>
   <si>
@@ -594,9 +552,6 @@
     <t>Cost optimization of OARO, COMRO, and LSRRO</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1044240293702</t>
-  </si>
-  <si>
     <t>Application of ceramic membrane and ion-exchange for the treatment of the flowback water from Marcellus shale gas production</t>
   </si>
   <si>
@@ -606,9 +561,6 @@
     <t>Experimental study of produced water treatment with ceramic membranes and desalination with ion exchange. A simple costing analysis is also included.</t>
   </si>
   <si>
-    <t>https://app.box.com/file/1045418745787</t>
-  </si>
-  <si>
     <t>Emerging desalination technologies: Current status, challenges and future trends</t>
   </si>
   <si>
@@ -616,9 +568,6 @@
   </si>
   <si>
     <t>Overview of recent developments in emerging desalination technologies</t>
-  </si>
-  <si>
-    <t>https://app.box.com/file/1054170297632</t>
   </si>
   <si>
     <t>Produced water pretreatment technologies are myriad. Notes on a variety of pretreatment technologies are collected here.</t>
@@ -3031,8 +2980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B45B649-91B1-4AA2-8B6E-BFBD2D0B9A8F}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4358,7 +4307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBAD0A05-BC9E-4385-A8AA-ED0DA016210A}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
@@ -4370,12 +4319,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>326</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4383,42 +4332,42 @@
     </row>
     <row r="5" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>330</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>332</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -4431,8 +4380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1831C72F-F70B-4757-8C3B-CC6E4644EE1C}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4458,303 +4407,250 @@
       <c r="D1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>129</v>
-      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>133</v>
-      </c>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>137</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>141</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>145</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>149</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>153</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>157</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>161</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>165</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>169</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>172</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>176</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>180</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>184</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>188</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="E17" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E11" r:id="rId1" xr:uid="{491EA42A-F546-4B66-B658-34C243536D3A}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{FC321445-9BCB-418E-A727-77A3D18EBBD9}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{7716B9D5-6E8D-4991-8452-69F4FE9285D1}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{6F74C19B-B7C5-4A80-B68A-5C46317E3AA6}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{3A3D7D8D-26BF-4C9D-BC72-E58D59DA8569}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{B5CF47F4-5E92-4D85-AC73-9C71EFAD60BC}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{B2319D99-A2E2-475F-A541-E3B65535F54C}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{93864E8F-72C0-443A-99AD-9A74DB9B1C7F}"/>
-    <hyperlink ref="E9" r:id="rId9" xr:uid="{A23A0241-8A8D-4CAE-B6E9-AD3690CF5C4C}"/>
-    <hyperlink ref="E10" r:id="rId10" xr:uid="{6C66F845-A2E7-43FD-B06C-AA0A6A389412}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{0E7C1985-ABE2-467E-8BF1-A9217CBEE094}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{5B2F5420-03CD-4429-8D5D-E1862F12E8A5}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{8486EC7E-11E2-4893-91B8-A854231C0FA7}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{07F0772D-13D3-4823-BA16-597C09A66C3C}"/>
-    <hyperlink ref="E16" r:id="rId15" xr:uid="{797C0F45-0BA0-40E0-B64A-7DF61725B512}"/>
-    <hyperlink ref="E17" r:id="rId16" xr:uid="{CBAEEEA2-6A08-4AB5-867A-3C187D5CF003}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4762,7 +4658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7EF076-EBBC-4CE1-A5AC-8B8AEB94A0FA}">
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -4779,12 +4675,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
-        <v>190</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4792,97 +4688,97 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>191</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>197</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>198</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>199</v>
+        <v>182</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>201</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>203</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>204</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -4895,7 +4791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7CC14E-CEFF-4451-9970-7DC1DCABB5CB}">
   <dimension ref="A1:A55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -4907,17 +4803,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>211</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4925,47 +4821,47 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4973,22 +4869,22 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -4996,12 +4892,12 @@
     </row>
     <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5009,22 +4905,22 @@
     </row>
     <row r="27" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5032,32 +4928,32 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5065,32 +4961,32 @@
     </row>
     <row r="41" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="2" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="4" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5098,37 +4994,37 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="4" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="4" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="2" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="2" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="2" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="2" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -5141,7 +5037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17371E9F-F6F3-4808-994B-CE0907EB1A7C}">
   <dimension ref="A1:A47"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -5153,12 +5049,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5166,52 +5062,52 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5219,22 +5115,22 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5242,32 +5138,32 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5275,47 +5171,47 @@
     </row>
     <row r="31" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5323,32 +5219,32 @@
     </row>
     <row r="42" spans="1:1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="2" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="2" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -5373,12 +5269,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5386,52 +5282,52 @@
     </row>
     <row r="5" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>281</v>
+        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>282</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>284</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5439,17 +5335,17 @@
     </row>
     <row r="17" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>288</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -5474,17 +5370,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5492,17 +5388,17 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -5527,12 +5423,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5540,17 +5436,17 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -5563,7 +5459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC151AA-A8EC-4E48-ACD0-5E33506F72C4}">
   <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -5575,12 +5471,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5588,32 +5484,32 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5621,37 +5517,37 @@
     </row>
     <row r="13" spans="1:1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>306</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5659,42 +5555,42 @@
     </row>
     <row r="22" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -5702,32 +5598,32 @@
     </row>
     <row r="32" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -5737,6 +5633,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DD81C0BC60B8F34E98292508E0F2290B" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b92cb22fc907bdfbb8c7cf2d0db3976">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ff8b091e-718a-46df-969f-fd7948bb87c1" xmlns:ns4="8d77a055-97e1-4cbf-923c-b2909e200c86" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d01377072be400b5330c5cd9a12685a9" ns3:_="" ns4:_="">
     <xsd:import namespace="ff8b091e-718a-46df-969f-fd7948bb87c1"/>
@@ -5977,15 +5882,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -5997,6 +5893,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5ADC133-0C3F-495C-B197-6AC2796CE080}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DAA0B34-8953-4E65-B5C9-28B52FC860E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6015,14 +5919,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5ADC133-0C3F-495C-B197-6AC2796CE080}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47070ADB-AF1A-48EC-8072-3E10F68AA33D}">
   <ds:schemaRefs>

</xml_diff>